<commit_message>
working on a text cycler
</commit_message>
<xml_diff>
--- a/parent_deaths.xlsx
+++ b/parent_deaths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$A$57</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$J$2</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -674,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,7 +1842,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G57"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>